<commit_message>
updated a bunch of things
</commit_message>
<xml_diff>
--- a/inst/extdata/demo_rainfall_1min_data.xlsx
+++ b/inst/extdata/demo_rainfall_1min_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="9" documentId="11_7BC79D5E344B00FC4EC4AEBD32F929AA8D3C4DD2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02C75BF1-2384-4D4A-BF2C-43849AE9D480}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="3615" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-23565" yWindow="2520" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -934,7 +934,7 @@
   <dimension ref="A1:B9350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75757,6 +75757,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
+    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e20f4bf570a29fdd68b6ac0ce9f23e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8333fcdd8157586878df4d15f204f2" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -76030,20 +76044,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
-    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59CA2C8-7811-4302-B3FE-FC4240DB0682}">
   <ds:schemaRefs>
@@ -76053,6 +76053,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91475E90-BE31-4491-A407-D9A4D3F0DE0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
+    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2564814-3CE5-4ADD-AE98-B927D4ED0189}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -76070,16 +76082,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91475E90-BE31-4491-A407-D9A4D3F0DE0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
-    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>